<commit_message>
Primeira versão na Sense
</commit_message>
<xml_diff>
--- a/ComandoUteisGit.xlsx
+++ b/ComandoUteisGit.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tassi\OneDrive\Desenvolvedor\Git\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Comando do Git " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Comando do Git</t>
   </si>
@@ -216,13 +211,37 @@
   </si>
   <si>
     <t>Verifica todas as atualizações feitas no repositório</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ls </t>
+  </si>
+  <si>
+    <t>lista os arquivos no repositorio</t>
+  </si>
+  <si>
+    <t>git tag</t>
+  </si>
+  <si>
+    <t>lista as tags dadas as versões. Util para quando cria-se versões finais novas</t>
+  </si>
+  <si>
+    <t>git checkout nomeDaTag</t>
+  </si>
+  <si>
+    <t>O git volta na versão respectiva a tag colocada</t>
+  </si>
+  <si>
+    <t>git diff nomeDaTag nomeDaOutraTag</t>
+  </si>
+  <si>
+    <t>Aqui é possíve comparar as diferenças entre as tags colocadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +265,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3D464D"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,11 +306,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -304,18 +344,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -330,12 +358,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C34"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Comando do Git" dataDxfId="4"/>
-    <tableColumn id="2" name="Ação" dataDxfId="3"/>
-    <tableColumn id="3" name="OBS" dataDxfId="2"/>
+    <tableColumn id="1" name="Comando do Git" dataDxfId="2"/>
+    <tableColumn id="2" name="Ação" dataDxfId="1"/>
+    <tableColumn id="3" name="OBS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +898,41 @@
         <v>63</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
colocando referencia de rebase
</commit_message>
<xml_diff>
--- a/ComandoUteisGit.xlsx
+++ b/ComandoUteisGit.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
   <si>
     <t>Comando do Git</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Ação</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/book/en/v2/Git-Branching-Rebasing</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,8 +461,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -479,11 +491,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -495,9 +520,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -512,7 +534,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -522,6 +562,26 @@
   <dxfs count="5">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -567,9 +627,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C53" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C53"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Comando do Git" dataDxfId="2"/>
-    <tableColumn id="2" name="Ação" dataDxfId="1"/>
-    <tableColumn id="3" name="OBS" dataDxfId="0"/>
+    <tableColumn id="1" name="Comando do Git" dataDxfId="0"/>
+    <tableColumn id="2" name="Ação" dataDxfId="2"/>
+    <tableColumn id="3" name="OBS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -830,7 +890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -840,9 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +914,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -865,7 +925,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -873,7 +933,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -881,7 +941,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -889,7 +949,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -897,7 +957,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -905,7 +965,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -913,7 +973,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -921,7 +981,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -932,7 +992,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -943,7 +1003,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -951,7 +1011,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -959,7 +1019,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -967,7 +1027,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -975,7 +1035,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -983,7 +1043,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -991,7 +1051,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -999,7 +1059,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1010,7 +1070,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1019,7 +1079,7 @@
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1027,7 +1087,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1035,7 +1095,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1043,7 +1103,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1051,7 +1111,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1062,7 +1122,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1071,258 +1131,258 @@
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="7"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="7"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1342,63 +1402,68 @@
       <c r="B57" s="10"/>
     </row>
     <row r="58" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>